<commit_message>
added populated columns for lat and long of ocean entry, and added placeholder columns for lat and long of sample site
</commit_message>
<xml_diff>
--- a/data/coho_coastw_pops_N_S.xlsx
+++ b/data/coho_coastw_pops_N_S.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="0" windowWidth="35640" windowHeight="26620" tabRatio="500"/>
+    <workbookView xWindow="5560" yWindow="460" windowWidth="29360" windowHeight="25440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="N-S by pop code" sheetId="5" r:id="rId1"/>
@@ -63,6 +63,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+lat and long ocean entry estimated from Google maps LGH 050316</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+lat and long ocean entry estimated from Google maps LGH 050316</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B2" authorId="0">
       <text>
         <r>
@@ -84,6 +132,54 @@
           </rPr>
           <t xml:space="preserve">
 n=2, drop?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+northern inlet of Elk River</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+northern inlet of Elk River</t>
         </r>
       </text>
     </comment>
@@ -282,6 +378,102 @@
         </r>
       </text>
     </comment>
+    <comment ref="F31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken at north end of Big Lagoon spit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken at north end of Big Lagoon spit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken at north end of Big Lagoon spit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken at north end of Big Lagoon spit</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B36" authorId="0">
       <text>
         <r>
@@ -303,6 +495,102 @@
           </rPr>
           <t xml:space="preserve">
 small n, omit from analysis?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F37" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken at mouth of Humboldt Bay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G37" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken at mouth of Humboldt Bay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken at mouth of Humboldt Bay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken at mouth of Humboldt Bay</t>
         </r>
       </text>
     </comment>
@@ -354,6 +642,78 @@
         </r>
       </text>
     </comment>
+    <comment ref="F68" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+mouth is just north of Point Arena</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F69" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+mouth is just north of Point Arena</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F70" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken where Walker Ck meets Tomales Bay</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B71" authorId="0">
       <text>
         <r>
@@ -375,6 +735,150 @@
           </rPr>
           <t xml:space="preserve">
 low n, to drop?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F71" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken where Lagunitas delta meets Tomales Bay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F72" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken where Lagunitas delta meets Tomales Bay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F73" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken where Lagunitas delta meets Tomales Bay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F74" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken where Lagunitas delta meets Tomales Bay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F75" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken where Lagunitas delta meets Tomales Bay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F76" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+coords taken where Lagunitas delta meets Tomales Bay</t>
         </r>
       </text>
     </comment>
@@ -762,7 +1266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="259">
   <si>
     <t>Noyo River</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -1567,6 +2071,21 @@
   </si>
   <si>
     <t>NS079</t>
+  </si>
+  <si>
+    <t>latitude_ocean_entry</t>
+  </si>
+  <si>
+    <t>longitude_ocean_entry</t>
+  </si>
+  <si>
+    <t>latitude_sample_site</t>
+  </si>
+  <si>
+    <t>longitude_sample_site</t>
+  </si>
+  <si>
+    <t>pending</t>
   </si>
 </sst>
 </file>
@@ -1703,7 +2222,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="289">
+  <cellStyleXfs count="399">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1993,8 +2512,118 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2045,8 +2674,14 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="289">
+  <cellStyles count="399">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2191,6 +2826,61 @@
     <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2335,6 +3025,61 @@
     <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2664,11 +3409,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2677,11 +3422,12 @@
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="30" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" style="30" customWidth="1"/>
+    <col min="8" max="9" width="18" style="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1">
+    <row r="1" spans="1:9" ht="18" customHeight="1">
       <c r="A1" s="21" t="s">
         <v>211</v>
       </c>
@@ -2697,8 +3443,20 @@
       <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="F1" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>143</v>
       </c>
@@ -2714,8 +3472,20 @@
       <c r="E2" s="7" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="F2" s="30">
+        <v>42.812247999999997</v>
+      </c>
+      <c r="G2" s="30">
+        <v>-124.53597600000001</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>144</v>
       </c>
@@ -2731,8 +3501,20 @@
       <c r="E3" s="7" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="F3" s="30">
+        <v>42.812247999999997</v>
+      </c>
+      <c r="G3" s="30">
+        <v>-124.53597600000001</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="15" t="s">
         <v>145</v>
       </c>
@@ -2748,8 +3530,20 @@
       <c r="E4" s="7" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="F4" s="30">
+        <v>42.419110000000003</v>
+      </c>
+      <c r="G4" s="30">
+        <v>-124.432435</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="15" t="s">
         <v>146</v>
       </c>
@@ -2765,8 +3559,20 @@
       <c r="E5" s="15" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="F5" s="30">
+        <v>42.419110000000003</v>
+      </c>
+      <c r="G5" s="30">
+        <v>-124.432435</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="15" t="s">
         <v>147</v>
       </c>
@@ -2782,8 +3588,20 @@
       <c r="E6" s="7" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="F6" s="30">
+        <v>42.419110000000003</v>
+      </c>
+      <c r="G6" s="30">
+        <v>-124.432435</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="15" t="s">
         <v>148</v>
       </c>
@@ -2799,8 +3617,20 @@
       <c r="E7" s="15" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="F7" s="30">
+        <v>42.419110000000003</v>
+      </c>
+      <c r="G7" s="30">
+        <v>-124.432435</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="15" t="s">
         <v>149</v>
       </c>
@@ -2816,8 +3646,20 @@
       <c r="E8" s="7" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="F8" s="30">
+        <v>42.419110000000003</v>
+      </c>
+      <c r="G8" s="30">
+        <v>-124.432435</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="15" t="s">
         <v>150</v>
       </c>
@@ -2833,8 +3675,20 @@
       <c r="E9" s="15" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="F9" s="30">
+        <v>42.419110000000003</v>
+      </c>
+      <c r="G9" s="30">
+        <v>-124.432435</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="15" t="s">
         <v>151</v>
       </c>
@@ -2850,8 +3704,20 @@
       <c r="E10" s="15" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="F10" s="30">
+        <v>42.043042999999997</v>
+      </c>
+      <c r="G10" s="30">
+        <v>-124.27168500000001</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="15" t="s">
         <v>152</v>
       </c>
@@ -2867,8 +3733,20 @@
       <c r="E11" s="15" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="F11" s="30">
+        <v>42.043042999999997</v>
+      </c>
+      <c r="G11" s="30">
+        <v>-124.27168500000001</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>153</v>
       </c>
@@ -2881,9 +3759,20 @@
       <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="F12" s="30">
+        <v>41.604196000000002</v>
+      </c>
+      <c r="G12" s="30">
+        <v>-124.101921</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>154</v>
       </c>
@@ -2897,9 +3786,20 @@
         <v>8</v>
       </c>
       <c r="E13" s="18"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="F13" s="30">
+        <v>41.604196000000002</v>
+      </c>
+      <c r="G13" s="30">
+        <v>-124.101921</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>155</v>
       </c>
@@ -2915,8 +3815,20 @@
       <c r="E14" s="3" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="F14" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G14" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I14" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="15" t="s">
         <v>156</v>
       </c>
@@ -2932,8 +3844,20 @@
       <c r="E15" s="3" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="F15" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G15" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I15" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="15" t="s">
         <v>157</v>
       </c>
@@ -2949,8 +3873,20 @@
       <c r="E16" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="F16" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G16" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I16" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="15" t="s">
         <v>158</v>
       </c>
@@ -2966,8 +3902,20 @@
       <c r="E17" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="F17" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G17" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I17" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="15" t="s">
         <v>159</v>
       </c>
@@ -2983,8 +3931,20 @@
       <c r="E18" s="3" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="F18" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G18" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I18" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="15" t="s">
         <v>160</v>
       </c>
@@ -3000,8 +3960,20 @@
       <c r="E19" s="3" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="F19" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G19" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I19" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="15" t="s">
         <v>161</v>
       </c>
@@ -3017,8 +3989,20 @@
       <c r="E20" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="F20" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G20" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="15" t="s">
         <v>162</v>
       </c>
@@ -3034,8 +4018,20 @@
       <c r="E21" s="3" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="F21" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G21" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I21" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="15" t="s">
         <v>163</v>
       </c>
@@ -3051,8 +4047,20 @@
       <c r="E22" s="3" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="F22" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G22" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H22" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I22" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>164</v>
       </c>
@@ -3068,8 +4076,20 @@
       <c r="E23" s="3" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="F23" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G23" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H23" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I23" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>165</v>
       </c>
@@ -3085,10 +4105,20 @@
       <c r="E24" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="F24" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G24" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>166</v>
       </c>
@@ -3104,8 +4134,20 @@
       <c r="E25" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="F25" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G25" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H25" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I25" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="15" t="s">
         <v>167</v>
       </c>
@@ -3121,8 +4163,20 @@
       <c r="E26" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="F26" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G26" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H26" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I26" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="15" t="s">
         <v>168</v>
       </c>
@@ -3138,8 +4192,20 @@
       <c r="E27" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="F27" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G27" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H27" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I27" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="15" t="s">
         <v>169</v>
       </c>
@@ -3155,8 +4221,20 @@
       <c r="E28" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="F28" s="30">
+        <v>41.542819999999999</v>
+      </c>
+      <c r="G28" s="30">
+        <v>-124.079177</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I28" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="15" t="s">
         <v>170</v>
       </c>
@@ -3172,8 +4250,20 @@
       <c r="E29" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="F29" s="30">
+        <v>41.292307999999998</v>
+      </c>
+      <c r="G29" s="30">
+        <v>-124.09187799999999</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="15" t="s">
         <v>171</v>
       </c>
@@ -3189,8 +4279,20 @@
       <c r="E30" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="F30" s="30">
+        <v>41.292307999999998</v>
+      </c>
+      <c r="G30" s="30">
+        <v>-124.09187799999999</v>
+      </c>
+      <c r="H30" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="15" t="s">
         <v>172</v>
       </c>
@@ -3206,8 +4308,20 @@
       <c r="E31" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="F31" s="30">
+        <v>41.209508999999997</v>
+      </c>
+      <c r="G31" s="30">
+        <v>-124.11702200000001</v>
+      </c>
+      <c r="H31" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I31" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="15" t="s">
         <v>173</v>
       </c>
@@ -3223,8 +4337,20 @@
       <c r="E32" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="F32" s="30">
+        <v>41.209508999999997</v>
+      </c>
+      <c r="G32" s="30">
+        <v>-124.11702200000001</v>
+      </c>
+      <c r="H32" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I32" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="15" t="s">
         <v>174</v>
       </c>
@@ -3240,8 +4366,20 @@
       <c r="E33" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="F33" s="30">
+        <v>41.027306000000003</v>
+      </c>
+      <c r="G33" s="30">
+        <v>-124.111926</v>
+      </c>
+      <c r="H33" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I33" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
         <v>175</v>
       </c>
@@ -3257,8 +4395,20 @@
       <c r="E34" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="F34" s="30">
+        <v>41.027306000000003</v>
+      </c>
+      <c r="G34" s="30">
+        <v>-124.111926</v>
+      </c>
+      <c r="H34" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I34" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
         <v>176</v>
       </c>
@@ -3274,8 +4424,20 @@
       <c r="E35" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="F35" s="30">
+        <v>40.972527999999997</v>
+      </c>
+      <c r="G35" s="30">
+        <v>-124.12290299999999</v>
+      </c>
+      <c r="H35" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I35" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
         <v>177</v>
       </c>
@@ -3291,10 +4453,20 @@
       <c r="E36" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="F36" s="30">
+        <v>40.972527999999997</v>
+      </c>
+      <c r="G36" s="30">
+        <v>-124.12290299999999</v>
+      </c>
+      <c r="H36" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I36" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="15" t="s">
         <v>178</v>
       </c>
@@ -3310,8 +4482,20 @@
       <c r="E37" s="3" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="F37" s="30">
+        <v>40.767724000000001</v>
+      </c>
+      <c r="G37" s="30">
+        <v>-124.242788</v>
+      </c>
+      <c r="H37" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I37" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="15" t="s">
         <v>179</v>
       </c>
@@ -3327,8 +4511,20 @@
       <c r="E38" s="3" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="F38" s="30">
+        <v>40.767724000000001</v>
+      </c>
+      <c r="G38" s="30">
+        <v>-124.242788</v>
+      </c>
+      <c r="H38" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I38" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="15" t="s">
         <v>180</v>
       </c>
@@ -3344,8 +4540,20 @@
       <c r="E39" s="3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="F39" s="30">
+        <v>40.649000999999998</v>
+      </c>
+      <c r="G39" s="30">
+        <v>-124.30950300000001</v>
+      </c>
+      <c r="H39" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I39" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="15" t="s">
         <v>181</v>
       </c>
@@ -3361,8 +4569,20 @@
       <c r="E40" s="3" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="F40" s="30">
+        <v>40.649000999999998</v>
+      </c>
+      <c r="G40" s="30">
+        <v>-124.30950300000001</v>
+      </c>
+      <c r="H40" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I40" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="15" t="s">
         <v>182</v>
       </c>
@@ -3378,8 +4598,20 @@
       <c r="E41" s="3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="F41" s="30">
+        <v>40.649000999999998</v>
+      </c>
+      <c r="G41" s="30">
+        <v>-124.30950300000001</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I41" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="15" t="s">
         <v>183</v>
       </c>
@@ -3392,8 +4624,20 @@
       <c r="D42" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="F42" s="3">
+        <v>40.302202999999999</v>
+      </c>
+      <c r="G42" s="3">
+        <v>-124.35406999999999</v>
+      </c>
+      <c r="H42" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I42" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="15" t="s">
         <v>191</v>
       </c>
@@ -3407,10 +4651,20 @@
         <v>22</v>
       </c>
       <c r="E43" s="6"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="F43" s="5">
+        <v>40.302202999999999</v>
+      </c>
+      <c r="G43" s="5">
+        <v>-124.35406999999999</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="15" t="s">
         <v>192</v>
       </c>
@@ -3426,8 +4680,20 @@
       <c r="E44" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="F44" s="30">
+        <v>39.736032000000002</v>
+      </c>
+      <c r="G44" s="30">
+        <v>-123.829384</v>
+      </c>
+      <c r="H44" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I44" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
         <v>193</v>
       </c>
@@ -3441,8 +4707,20 @@
         <v>25</v>
       </c>
       <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="F45" s="30">
+        <v>39.651716</v>
+      </c>
+      <c r="G45" s="30">
+        <v>-123.785082</v>
+      </c>
+      <c r="H45" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I45" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
         <v>194</v>
       </c>
@@ -3456,8 +4734,20 @@
         <v>25</v>
       </c>
       <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="F46" s="30">
+        <v>39.651716</v>
+      </c>
+      <c r="G46" s="30">
+        <v>-123.785082</v>
+      </c>
+      <c r="H46" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I46" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
         <v>195</v>
       </c>
@@ -3473,8 +4763,20 @@
       <c r="E47" s="3" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="F47" s="30">
+        <v>39.553401999999998</v>
+      </c>
+      <c r="G47" s="30">
+        <v>-123.76682599999999</v>
+      </c>
+      <c r="H47" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I47" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="15" t="s">
         <v>196</v>
       </c>
@@ -3490,10 +4792,20 @@
       <c r="E48" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="F48" s="30">
+        <v>39.553401999999998</v>
+      </c>
+      <c r="G48" s="30">
+        <v>-123.76682599999999</v>
+      </c>
+      <c r="H48" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I48" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="15" t="s">
         <v>222</v>
       </c>
@@ -3509,8 +4821,20 @@
       <c r="E49" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="F49" s="30">
+        <v>39.553401999999998</v>
+      </c>
+      <c r="G49" s="30">
+        <v>-123.76682599999999</v>
+      </c>
+      <c r="H49" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I49" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="15" t="s">
         <v>223</v>
       </c>
@@ -3526,8 +4850,20 @@
       <c r="E50" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="F50" s="30">
+        <v>39.553401999999998</v>
+      </c>
+      <c r="G50" s="30">
+        <v>-123.76682599999999</v>
+      </c>
+      <c r="H50" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I50" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="15" t="s">
         <v>224</v>
       </c>
@@ -3541,8 +4877,20 @@
         <v>27</v>
       </c>
       <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="F51" s="30">
+        <v>39.459125</v>
+      </c>
+      <c r="G51" s="30">
+        <v>-123.80941199999999</v>
+      </c>
+      <c r="H51" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I51" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="15" t="s">
         <v>225</v>
       </c>
@@ -3556,8 +4904,20 @@
         <v>27</v>
       </c>
       <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="F52" s="30">
+        <v>39.459125</v>
+      </c>
+      <c r="G52" s="30">
+        <v>-123.80941199999999</v>
+      </c>
+      <c r="H52" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I52" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="15" t="s">
         <v>226</v>
       </c>
@@ -3573,8 +4933,20 @@
       <c r="E53" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="F53" s="30">
+        <v>39.427914000000001</v>
+      </c>
+      <c r="G53" s="30">
+        <v>-123.810671</v>
+      </c>
+      <c r="H53" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I53" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="15" t="s">
         <v>227</v>
       </c>
@@ -3590,8 +4962,20 @@
       <c r="E54" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="F54" s="30">
+        <v>39.427914000000001</v>
+      </c>
+      <c r="G54" s="30">
+        <v>-123.810671</v>
+      </c>
+      <c r="H54" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I54" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" s="15" t="s">
         <v>228</v>
       </c>
@@ -3605,8 +4989,20 @@
         <v>1</v>
       </c>
       <c r="E55" s="3"/>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="F55" s="30">
+        <v>39.361863999999997</v>
+      </c>
+      <c r="G55" s="30">
+        <v>-123.81754599999999</v>
+      </c>
+      <c r="H55" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I55" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
         <v>229</v>
       </c>
@@ -3620,8 +5016,20 @@
         <v>1</v>
       </c>
       <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="F56" s="30">
+        <v>39.361863999999997</v>
+      </c>
+      <c r="G56" s="30">
+        <v>-123.81754599999999</v>
+      </c>
+      <c r="H56" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I56" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
         <v>230</v>
       </c>
@@ -3637,8 +5045,20 @@
       <c r="E57" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="F57" s="30">
+        <v>39.302027000000002</v>
+      </c>
+      <c r="G57" s="30">
+        <v>-123.794493</v>
+      </c>
+      <c r="H57" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I57" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
         <v>231</v>
       </c>
@@ -3654,8 +5074,20 @@
       <c r="E58" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="F58" s="30">
+        <v>39.302027000000002</v>
+      </c>
+      <c r="G58" s="30">
+        <v>-123.794493</v>
+      </c>
+      <c r="H58" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I58" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" s="15" t="s">
         <v>232</v>
       </c>
@@ -3669,8 +5101,20 @@
         <v>20</v>
       </c>
       <c r="E59" s="3"/>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="F59" s="30">
+        <v>39.273693000000002</v>
+      </c>
+      <c r="G59" s="30">
+        <v>-123.791837</v>
+      </c>
+      <c r="H59" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I59" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" s="15" t="s">
         <v>233</v>
       </c>
@@ -3684,8 +5128,20 @@
         <v>20</v>
       </c>
       <c r="E60" s="3"/>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="F60" s="30">
+        <v>39.273693000000002</v>
+      </c>
+      <c r="G60" s="30">
+        <v>-123.791837</v>
+      </c>
+      <c r="H60" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I60" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="15" t="s">
         <v>234</v>
       </c>
@@ -3699,8 +5155,20 @@
         <v>4</v>
       </c>
       <c r="E61" s="3"/>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="F61" s="30">
+        <v>39.226984999999999</v>
+      </c>
+      <c r="G61" s="30">
+        <v>-123.770308</v>
+      </c>
+      <c r="H61" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I61" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="15" t="s">
         <v>235</v>
       </c>
@@ -3714,10 +5182,20 @@
         <v>4</v>
       </c>
       <c r="E62" s="18"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="F62" s="30">
+        <v>39.226984999999999</v>
+      </c>
+      <c r="G62" s="30">
+        <v>-123.770308</v>
+      </c>
+      <c r="H62" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I62" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="15" t="s">
         <v>236</v>
       </c>
@@ -3731,8 +5209,20 @@
         <v>5</v>
       </c>
       <c r="E63" s="3"/>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="F63" s="30">
+        <v>39.215594000000003</v>
+      </c>
+      <c r="G63" s="30">
+        <v>-123.769274</v>
+      </c>
+      <c r="H63" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I63" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" s="15" t="s">
         <v>237</v>
       </c>
@@ -3746,8 +5236,20 @@
         <v>5</v>
       </c>
       <c r="E64" s="3"/>
-    </row>
-    <row r="65" spans="1:7">
+      <c r="F64" s="30">
+        <v>39.215594000000003</v>
+      </c>
+      <c r="G64" s="30">
+        <v>-123.769274</v>
+      </c>
+      <c r="H64" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I64" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" s="15" t="s">
         <v>238</v>
       </c>
@@ -3763,8 +5265,20 @@
       <c r="E65" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="F65" s="30">
+        <v>39.191763000000002</v>
+      </c>
+      <c r="G65" s="30">
+        <v>-123.761134</v>
+      </c>
+      <c r="H65" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I65" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="15" t="s">
         <v>239</v>
       </c>
@@ -3780,8 +5294,20 @@
       <c r="E66" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="F66" s="30">
+        <v>39.191763000000002</v>
+      </c>
+      <c r="G66" s="30">
+        <v>-123.761134</v>
+      </c>
+      <c r="H66" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I66" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
         <v>240</v>
       </c>
@@ -3797,8 +5323,20 @@
       <c r="E67" s="15" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="68" spans="1:7">
+      <c r="F67" s="30">
+        <v>39.191763000000002</v>
+      </c>
+      <c r="G67" s="30">
+        <v>-123.761134</v>
+      </c>
+      <c r="H67" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I67" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
         <v>241</v>
       </c>
@@ -3814,8 +5352,20 @@
       <c r="E68" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="69" spans="1:7">
+      <c r="F68" s="30">
+        <v>38.954810000000002</v>
+      </c>
+      <c r="G68" s="30">
+        <v>-123.733526</v>
+      </c>
+      <c r="H68" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I68" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" s="1" t="s">
         <v>242</v>
       </c>
@@ -3831,8 +5381,20 @@
       <c r="E69" s="7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="70" spans="1:7">
+      <c r="F69" s="30">
+        <v>38.954810000000002</v>
+      </c>
+      <c r="G69" s="30">
+        <v>-123.733526</v>
+      </c>
+      <c r="H69" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I69" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70" s="15" t="s">
         <v>243</v>
       </c>
@@ -3846,8 +5408,20 @@
         <v>136</v>
       </c>
       <c r="E70" s="15"/>
-    </row>
-    <row r="71" spans="1:7">
+      <c r="F70" s="30">
+        <v>38.209601999999997</v>
+      </c>
+      <c r="G70" s="30">
+        <v>-122.92983</v>
+      </c>
+      <c r="H70" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I70" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" s="15" t="s">
         <v>244</v>
       </c>
@@ -3861,8 +5435,20 @@
         <v>32</v>
       </c>
       <c r="E71" s="3"/>
-    </row>
-    <row r="72" spans="1:7">
+      <c r="F71" s="30">
+        <v>38.089637000000003</v>
+      </c>
+      <c r="G71" s="30">
+        <v>-122.833217</v>
+      </c>
+      <c r="H71" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I71" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72" s="15" t="s">
         <v>245</v>
       </c>
@@ -3876,8 +5462,20 @@
         <v>32</v>
       </c>
       <c r="E72" s="3"/>
-    </row>
-    <row r="73" spans="1:7">
+      <c r="F72" s="30">
+        <v>38.089637000000003</v>
+      </c>
+      <c r="G72" s="30">
+        <v>-122.833217</v>
+      </c>
+      <c r="H72" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I72" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" s="15" t="s">
         <v>246</v>
       </c>
@@ -3893,8 +5491,20 @@
       <c r="E73" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="74" spans="1:7">
+      <c r="F73" s="30">
+        <v>38.089637000000003</v>
+      </c>
+      <c r="G73" s="30">
+        <v>-122.833217</v>
+      </c>
+      <c r="H73" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I73" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74" s="15" t="s">
         <v>247</v>
       </c>
@@ -3910,8 +5520,20 @@
       <c r="E74" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="75" spans="1:7">
+      <c r="F74" s="30">
+        <v>38.089637000000003</v>
+      </c>
+      <c r="G74" s="30">
+        <v>-122.833217</v>
+      </c>
+      <c r="H74" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I74" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75" s="15" t="s">
         <v>248</v>
       </c>
@@ -3927,8 +5549,20 @@
       <c r="E75" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="76" spans="1:7">
+      <c r="F75" s="30">
+        <v>38.089637000000003</v>
+      </c>
+      <c r="G75" s="30">
+        <v>-122.833217</v>
+      </c>
+      <c r="H75" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I75" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76" s="15" t="s">
         <v>249</v>
       </c>
@@ -3944,8 +5578,20 @@
       <c r="E76" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="77" spans="1:7">
+      <c r="F76" s="30">
+        <v>38.089637000000003</v>
+      </c>
+      <c r="G76" s="30">
+        <v>-122.833217</v>
+      </c>
+      <c r="H76" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I76" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77" s="15" t="s">
         <v>250</v>
       </c>
@@ -3959,8 +5605,20 @@
         <v>16</v>
       </c>
       <c r="E77" s="3"/>
-    </row>
-    <row r="78" spans="1:7">
+      <c r="F77" s="30">
+        <v>37.859591999999999</v>
+      </c>
+      <c r="G77" s="30">
+        <v>-122.578053</v>
+      </c>
+      <c r="H77" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I77" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78" s="1" t="s">
         <v>251</v>
       </c>
@@ -3974,8 +5632,20 @@
         <v>16</v>
       </c>
       <c r="E78" s="3"/>
-    </row>
-    <row r="79" spans="1:7" s="15" customFormat="1">
+      <c r="F78" s="30">
+        <v>37.859591999999999</v>
+      </c>
+      <c r="G78" s="30">
+        <v>-122.578053</v>
+      </c>
+      <c r="H78" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I78" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" s="15" customFormat="1">
       <c r="A79" s="1" t="s">
         <v>252</v>
       </c>
@@ -3989,8 +5659,20 @@
         <v>35</v>
       </c>
       <c r="E79" s="3"/>
-    </row>
-    <row r="80" spans="1:7" s="15" customFormat="1">
+      <c r="F79" s="3">
+        <v>37.041151999999997</v>
+      </c>
+      <c r="G79" s="3">
+        <v>-122.230897</v>
+      </c>
+      <c r="H79" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I79" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" s="15" customFormat="1">
       <c r="A80" s="1" t="s">
         <v>253</v>
       </c>
@@ -4004,8 +5686,18 @@
         <v>35</v>
       </c>
       <c r="E80" s="18"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
+      <c r="F80" s="3">
+        <v>37.041151999999997</v>
+      </c>
+      <c r="G80" s="3">
+        <v>-122.230897</v>
+      </c>
+      <c r="H80" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="I80" s="30" t="s">
+        <v>258</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added lat-longs of sample sites (third attempt to commit)
</commit_message>
<xml_diff>
--- a/data/coho_coastw_pops_N_S.xlsx
+++ b/data/coho_coastw_pops_N_S.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="460" windowWidth="29360" windowHeight="25440" tabRatio="500"/>
+    <workbookView xWindow="600" yWindow="160" windowWidth="26900" windowHeight="25860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="N-S by pop code" sheetId="5" r:id="rId1"/>
@@ -111,6 +111,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+data from field collectors, compiled by Kerrie Pipal</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+data from field collectors, compiled by Kerrie Pipal</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B2" authorId="0">
       <text>
         <r>
@@ -594,7 +642,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E47" authorId="0">
+    <comment ref="H40" authorId="0">
       <text>
         <r>
           <rPr>
@@ -614,11 +662,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Little North Fork or Lower North Fork?</t>
+per Tommy on TRT data, two HT sites were almost on top of each other, so treat as a single pop.  EHTa and EHUa should be combined for most analysis 050616</t>
         </r>
       </text>
     </comment>
-    <comment ref="E48" authorId="0">
+    <comment ref="I40" authorId="0">
       <text>
         <r>
           <rPr>
@@ -638,7 +686,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Little North Fork or Lower North Fork?</t>
+per Tommy on TRT data, two HT sites were almost on top of each other, so treat as a single pop.  EHTa and EHUa should be combined for most analysis 050616</t>
         </r>
       </text>
     </comment>
@@ -1266,7 +1314,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="266">
   <si>
     <t>Noyo River</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -2085,14 +2133,38 @@
     <t>longitude_sample_site</t>
   </si>
   <si>
-    <t>pending</t>
+    <t>-124.086242</t>
+  </si>
+  <si>
+    <t>Upper Mattole River Whitethorn</t>
+  </si>
+  <si>
+    <t>Mattole River</t>
+  </si>
+  <si>
+    <t>Upper Mattole River</t>
+  </si>
+  <si>
+    <t>Little North Fork</t>
+  </si>
+  <si>
+    <t>South Fork</t>
+  </si>
+  <si>
+    <t>North Fork</t>
+  </si>
+  <si>
+    <t>Rogue River Upper</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
+  </numFmts>
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -2183,6 +2255,11 @@
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2222,7 +2299,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="399">
+  <cellStyleXfs count="419">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2622,8 +2699,28 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2677,11 +2774,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="399">
+  <cellStyles count="419">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2881,6 +2999,16 @@
     <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3080,6 +3208,16 @@
     <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3411,20 +3549,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41:G41"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="30" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" style="30" customWidth="1"/>
-    <col min="8" max="9" width="18" style="31" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="7" width="13.42578125" style="30" customWidth="1"/>
+    <col min="8" max="9" width="16.42578125" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" customHeight="1">
@@ -3478,11 +3615,11 @@
       <c r="G2" s="30">
         <v>-124.53597600000001</v>
       </c>
-      <c r="H2" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>258</v>
+      <c r="H2" s="30">
+        <v>42.738500000000002</v>
+      </c>
+      <c r="I2" s="30">
+        <v>-124.40089999999999</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3507,11 +3644,11 @@
       <c r="G3" s="30">
         <v>-124.53597600000001</v>
       </c>
-      <c r="H3" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I3" s="30" t="s">
-        <v>258</v>
+      <c r="H3" s="30">
+        <v>42.69885</v>
+      </c>
+      <c r="I3" s="30">
+        <v>-124.28699</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3525,7 +3662,7 @@
         <v>142</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>115</v>
+        <v>265</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>118</v>
@@ -3536,11 +3673,11 @@
       <c r="G4" s="30">
         <v>-124.432435</v>
       </c>
-      <c r="H4" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>258</v>
+      <c r="H4" s="30">
+        <v>42.709449999999997</v>
+      </c>
+      <c r="I4" s="30">
+        <v>-122.74825</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3554,7 +3691,7 @@
         <v>142</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>115</v>
+        <v>265</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>119</v>
@@ -3565,11 +3702,11 @@
       <c r="G5" s="30">
         <v>-124.432435</v>
       </c>
-      <c r="H5" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>258</v>
+      <c r="H5" s="30">
+        <v>42.649880000000003</v>
+      </c>
+      <c r="I5" s="30">
+        <v>-123.04346</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3594,11 +3731,11 @@
       <c r="G6" s="30">
         <v>-124.432435</v>
       </c>
-      <c r="H6" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>258</v>
+      <c r="H6" s="30">
+        <v>42.48574</v>
+      </c>
+      <c r="I6" s="30">
+        <v>-124.38927</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3612,7 +3749,7 @@
         <v>142</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>115</v>
+        <v>217</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>116</v>
@@ -3623,11 +3760,11 @@
       <c r="G7" s="30">
         <v>-124.432435</v>
       </c>
-      <c r="H7" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I7" s="30" t="s">
-        <v>258</v>
+      <c r="H7" s="30">
+        <v>42.506889999999999</v>
+      </c>
+      <c r="I7" s="30">
+        <v>-123.62509</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3646,17 +3783,17 @@
       <c r="E8" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="3">
         <v>42.419110000000003</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="3">
         <v>-124.432435</v>
       </c>
-      <c r="H8" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I8" s="30" t="s">
-        <v>258</v>
+      <c r="H8" s="3">
+        <v>42.139969999999998</v>
+      </c>
+      <c r="I8" s="3">
+        <v>-123.45679</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3681,11 +3818,11 @@
       <c r="G9" s="30">
         <v>-124.432435</v>
       </c>
-      <c r="H9" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I9" s="30" t="s">
-        <v>258</v>
+      <c r="H9" s="30">
+        <v>42.389200000000002</v>
+      </c>
+      <c r="I9" s="30">
+        <v>-123.553403</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3710,11 +3847,11 @@
       <c r="G10" s="30">
         <v>-124.27168500000001</v>
       </c>
-      <c r="H10" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I10" s="30" t="s">
-        <v>258</v>
+      <c r="H10" s="30">
+        <v>42.115989999999996</v>
+      </c>
+      <c r="I10" s="30">
+        <v>-124.18497000000001</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3739,11 +3876,11 @@
       <c r="G11" s="30">
         <v>-124.27168500000001</v>
       </c>
-      <c r="H11" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I11" s="30" t="s">
-        <v>258</v>
+      <c r="H11" s="7">
+        <v>42.06176</v>
+      </c>
+      <c r="I11" s="7">
+        <v>-124.21621</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -3765,11 +3902,11 @@
       <c r="G12" s="30">
         <v>-124.101921</v>
       </c>
-      <c r="H12" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>258</v>
+      <c r="H12" s="36">
+        <v>41.612006999999998</v>
+      </c>
+      <c r="I12" s="36">
+        <v>-124.09543103367299</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -3792,10 +3929,10 @@
       <c r="G13" s="30">
         <v>-124.101921</v>
       </c>
-      <c r="H13" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I13" s="30" t="s">
+      <c r="H13" s="32">
+        <v>41.647773000000001</v>
+      </c>
+      <c r="I13" s="33" t="s">
         <v>258</v>
       </c>
     </row>
@@ -3821,11 +3958,11 @@
       <c r="G14" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H14" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I14" s="30" t="s">
-        <v>258</v>
+      <c r="H14" s="35">
+        <v>41.538673000000003</v>
+      </c>
+      <c r="I14" s="35">
+        <v>-123.827192707953</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3850,11 +3987,11 @@
       <c r="G15" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H15" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I15" s="30" t="s">
-        <v>258</v>
+      <c r="H15" s="34">
+        <v>41.514270000000003</v>
+      </c>
+      <c r="I15" s="34">
+        <v>-123.83504000000001</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3879,11 +4016,11 @@
       <c r="G16" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H16" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I16" s="30" t="s">
-        <v>258</v>
+      <c r="H16" s="35">
+        <v>41.490836999999999</v>
+      </c>
+      <c r="I16" s="35">
+        <v>-124.00763020422001</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -3908,11 +4045,11 @@
       <c r="G17" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H17" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I17" s="30" t="s">
-        <v>258</v>
+      <c r="H17" s="7">
+        <v>41.49109</v>
+      </c>
+      <c r="I17" s="7">
+        <v>-124.00812999999999</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -3937,11 +4074,11 @@
       <c r="G18" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H18" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I18" s="30" t="s">
-        <v>258</v>
+      <c r="H18" s="35">
+        <v>41.724341000000003</v>
+      </c>
+      <c r="I18" s="35">
+        <v>-123.009882885439</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -3966,11 +4103,11 @@
       <c r="G19" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H19" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I19" s="30" t="s">
-        <v>258</v>
+      <c r="H19" s="30">
+        <v>41.724341843859499</v>
+      </c>
+      <c r="I19" s="30">
+        <v>-123.009882885439</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -3995,11 +4132,11 @@
       <c r="G20" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H20" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>258</v>
+      <c r="H20" s="35">
+        <v>41.948107999999998</v>
+      </c>
+      <c r="I20" s="35">
+        <v>-122.841068728697</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -4024,11 +4161,11 @@
       <c r="G21" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H21" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I21" s="30" t="s">
-        <v>258</v>
+      <c r="H21" s="35">
+        <v>41.827376999999998</v>
+      </c>
+      <c r="I21" s="35">
+        <v>-122.59430958091799</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -4053,11 +4190,11 @@
       <c r="G22" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H22" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I22" s="30" t="s">
-        <v>258</v>
+      <c r="H22" s="30">
+        <v>41.827377692233497</v>
+      </c>
+      <c r="I22" s="30">
+        <v>-122.594309580917</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -4082,11 +4219,11 @@
       <c r="G23" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H23" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I23" s="30" t="s">
-        <v>258</v>
+      <c r="H23" s="35">
+        <v>41.827376999999998</v>
+      </c>
+      <c r="I23" s="35">
+        <v>-122.59430958091799</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -4111,11 +4248,11 @@
       <c r="G24" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H24" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I24" s="30" t="s">
-        <v>258</v>
+      <c r="H24" s="30">
+        <v>41.827377692233497</v>
+      </c>
+      <c r="I24" s="30">
+        <v>-122.594309580917</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -4140,11 +4277,11 @@
       <c r="G25" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H25" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I25" s="30" t="s">
-        <v>258</v>
+      <c r="H25" s="37">
+        <v>40.897407000000001</v>
+      </c>
+      <c r="I25" s="37">
+        <v>-123.566696743883</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -4169,11 +4306,11 @@
       <c r="G26" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H26" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I26" s="30" t="s">
-        <v>258</v>
+      <c r="H26" s="30">
+        <v>40.895730999999998</v>
+      </c>
+      <c r="I26" s="30">
+        <v>-123.56357199999999</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -4198,11 +4335,11 @@
       <c r="G27" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H27" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I27" s="30" t="s">
-        <v>258</v>
+      <c r="H27" s="35">
+        <v>40.659545999999999</v>
+      </c>
+      <c r="I27" s="35">
+        <v>-123.029408706826</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -4227,11 +4364,11 @@
       <c r="G28" s="30">
         <v>-124.079177</v>
       </c>
-      <c r="H28" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I28" s="30" t="s">
-        <v>258</v>
+      <c r="H28" s="30">
+        <v>40.6595462422029</v>
+      </c>
+      <c r="I28" s="30">
+        <v>-123.029473</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -4256,11 +4393,11 @@
       <c r="G29" s="30">
         <v>-124.09187799999999</v>
       </c>
-      <c r="H29" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I29" s="30" t="s">
-        <v>258</v>
+      <c r="H29" s="37">
+        <v>41.406913000000003</v>
+      </c>
+      <c r="I29" s="37">
+        <v>-124.03122953915801</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -4285,11 +4422,11 @@
       <c r="G30" s="30">
         <v>-124.09187799999999</v>
       </c>
-      <c r="H30" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I30" s="30" t="s">
-        <v>258</v>
+      <c r="H30" s="30">
+        <v>41.406912670925003</v>
+      </c>
+      <c r="I30" s="30">
+        <v>-124.03122953916299</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -4314,11 +4451,11 @@
       <c r="G31" s="30">
         <v>-124.11702200000001</v>
       </c>
-      <c r="H31" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I31" s="30" t="s">
-        <v>258</v>
+      <c r="H31" s="37">
+        <v>41.141115999999997</v>
+      </c>
+      <c r="I31" s="37">
+        <v>-124.092792708061</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -4343,11 +4480,11 @@
       <c r="G32" s="30">
         <v>-124.11702200000001</v>
       </c>
-      <c r="H32" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I32" s="30" t="s">
-        <v>258</v>
+      <c r="H32" s="30">
+        <v>41.141115519451503</v>
+      </c>
+      <c r="I32" s="30">
+        <v>-124.092792708066</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -4372,11 +4509,11 @@
       <c r="G33" s="30">
         <v>-124.111926</v>
       </c>
-      <c r="H33" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I33" s="30" t="s">
-        <v>258</v>
+      <c r="H33" s="36">
+        <v>41.026094000000001</v>
+      </c>
+      <c r="I33" s="36">
+        <v>-123.995455266097</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -4401,11 +4538,11 @@
       <c r="G34" s="30">
         <v>-124.111926</v>
       </c>
-      <c r="H34" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I34" s="30" t="s">
-        <v>258</v>
+      <c r="H34" s="30">
+        <v>41.026084341568698</v>
+      </c>
+      <c r="I34" s="30">
+        <v>-123.99545659695799</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -4430,11 +4567,11 @@
       <c r="G35" s="30">
         <v>-124.12290299999999</v>
       </c>
-      <c r="H35" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I35" s="30" t="s">
-        <v>258</v>
+      <c r="H35" s="36">
+        <v>40.868766999999998</v>
+      </c>
+      <c r="I35" s="36">
+        <v>-123.961258081978</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -4459,11 +4596,11 @@
       <c r="G36" s="30">
         <v>-124.12290299999999</v>
       </c>
-      <c r="H36" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I36" s="30" t="s">
-        <v>258</v>
+      <c r="H36" s="30">
+        <v>40.868759343637798</v>
+      </c>
+      <c r="I36" s="30">
+        <v>-123.96125839195</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -4488,11 +4625,11 @@
       <c r="G37" s="30">
         <v>-124.242788</v>
       </c>
-      <c r="H37" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I37" s="30" t="s">
-        <v>258</v>
+      <c r="H37" s="37">
+        <v>40.733694</v>
+      </c>
+      <c r="I37" s="37">
+        <v>-124.048557319376</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -4517,11 +4654,11 @@
       <c r="G38" s="30">
         <v>-124.242788</v>
       </c>
-      <c r="H38" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I38" s="30" t="s">
-        <v>258</v>
+      <c r="H38" s="30">
+        <v>40.733693246691601</v>
+      </c>
+      <c r="I38" s="30">
+        <v>-124.048557319381</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -4546,11 +4683,11 @@
       <c r="G39" s="30">
         <v>-124.30950300000001</v>
       </c>
-      <c r="H39" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I39" s="30" t="s">
-        <v>258</v>
+      <c r="H39" s="37">
+        <v>39.739350000000002</v>
+      </c>
+      <c r="I39" s="37">
+        <v>-123.719786158689</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -4575,11 +4712,11 @@
       <c r="G40" s="30">
         <v>-124.30950300000001</v>
       </c>
-      <c r="H40" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I40" s="30" t="s">
-        <v>258</v>
+      <c r="H40" s="38">
+        <v>39.739350000000002</v>
+      </c>
+      <c r="I40" s="38">
+        <v>-123.719786158689</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -4604,11 +4741,11 @@
       <c r="G41" s="30">
         <v>-124.30950300000001</v>
       </c>
-      <c r="H41" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I41" s="30" t="s">
-        <v>258</v>
+      <c r="H41" s="30">
+        <v>39.373964999999998</v>
+      </c>
+      <c r="I41" s="30">
+        <v>-123.719786</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -4622,7 +4759,10 @@
         <v>140</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>22</v>
+        <v>260</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>261</v>
       </c>
       <c r="F42" s="3">
         <v>40.302202999999999</v>
@@ -4630,11 +4770,11 @@
       <c r="G42" s="3">
         <v>-124.35406999999999</v>
       </c>
-      <c r="H42" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I42" s="30" t="s">
-        <v>258</v>
+      <c r="H42" s="35">
+        <v>39.993645000000001</v>
+      </c>
+      <c r="I42" s="35">
+        <v>-123.924254484123</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -4650,18 +4790,20 @@
       <c r="D43" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E43" s="6"/>
+      <c r="E43" s="6" t="s">
+        <v>259</v>
+      </c>
       <c r="F43" s="5">
         <v>40.302202999999999</v>
       </c>
       <c r="G43" s="5">
         <v>-124.35406999999999</v>
       </c>
-      <c r="H43" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>258</v>
+      <c r="H43" s="5">
+        <v>40.008785000000003</v>
+      </c>
+      <c r="I43" s="5">
+        <v>-123.93082699999999</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -4686,11 +4828,11 @@
       <c r="G44" s="30">
         <v>-123.829384</v>
       </c>
-      <c r="H44" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I44" s="30" t="s">
-        <v>258</v>
+      <c r="H44" s="37">
+        <v>39.737169000000002</v>
+      </c>
+      <c r="I44" s="37">
+        <v>-123.811457138802</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -4713,11 +4855,11 @@
       <c r="G45" s="30">
         <v>-123.785082</v>
       </c>
-      <c r="H45" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I45" s="30" t="s">
-        <v>258</v>
+      <c r="H45" s="37">
+        <v>39.646847999999999</v>
+      </c>
+      <c r="I45" s="37">
+        <v>-123.739059359408</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -4740,11 +4882,11 @@
       <c r="G46" s="30">
         <v>-123.785082</v>
       </c>
-      <c r="H46" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I46" s="30" t="s">
-        <v>258</v>
+      <c r="H46" s="30">
+        <v>39.6468482090145</v>
+      </c>
+      <c r="I46" s="30">
+        <v>-123.739059359411</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -4761,7 +4903,7 @@
         <v>26</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
       <c r="F47" s="30">
         <v>39.553401999999998</v>
@@ -4769,11 +4911,11 @@
       <c r="G47" s="30">
         <v>-123.76682599999999</v>
       </c>
-      <c r="H47" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I47" s="30" t="s">
-        <v>258</v>
+      <c r="H47" s="37">
+        <v>39.593316999999999</v>
+      </c>
+      <c r="I47" s="37">
+        <v>-123.71178554974099</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -4790,7 +4932,7 @@
         <v>26</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
       <c r="F48" s="30">
         <v>39.553401999999998</v>
@@ -4798,11 +4940,11 @@
       <c r="G48" s="30">
         <v>-123.76682599999999</v>
       </c>
-      <c r="H48" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I48" s="30" t="s">
-        <v>258</v>
+      <c r="H48" s="30">
+        <v>39.593317417398701</v>
+      </c>
+      <c r="I48" s="30">
+        <v>-123.71178554974399</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -4827,11 +4969,11 @@
       <c r="G49" s="30">
         <v>-123.76682599999999</v>
       </c>
-      <c r="H49" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I49" s="30" t="s">
-        <v>258</v>
+      <c r="H49" s="30">
+        <v>39.515115999999999</v>
+      </c>
+      <c r="I49" s="30">
+        <v>-123.707942</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -4856,11 +4998,11 @@
       <c r="G50" s="30">
         <v>-123.76682599999999</v>
       </c>
-      <c r="H50" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I50" s="30" t="s">
-        <v>258</v>
+      <c r="H50" s="30">
+        <v>39.503129000000001</v>
+      </c>
+      <c r="I50" s="30">
+        <v>-123.610786</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -4883,11 +5025,11 @@
       <c r="G51" s="30">
         <v>-123.80941199999999</v>
       </c>
-      <c r="H51" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I51" s="30" t="s">
-        <v>258</v>
+      <c r="H51" s="37">
+        <v>39.467663000000002</v>
+      </c>
+      <c r="I51" s="37">
+        <v>-123.72560470636201</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -4910,11 +5052,11 @@
       <c r="G52" s="30">
         <v>-123.80941199999999</v>
       </c>
-      <c r="H52" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I52" s="30" t="s">
-        <v>258</v>
+      <c r="H52" s="30">
+        <v>39.467663053255897</v>
+      </c>
+      <c r="I52" s="30">
+        <v>-123.725604706365</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -4939,11 +5081,11 @@
       <c r="G53" s="30">
         <v>-123.810671</v>
       </c>
-      <c r="H53" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I53" s="30" t="s">
-        <v>258</v>
+      <c r="H53" s="37">
+        <v>39.383845000000001</v>
+      </c>
+      <c r="I53" s="37">
+        <v>-123.673425752428</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -4968,11 +5110,11 @@
       <c r="G54" s="30">
         <v>-123.810671</v>
       </c>
-      <c r="H54" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I54" s="30" t="s">
-        <v>258</v>
+      <c r="H54" s="30">
+        <v>39.3838452552584</v>
+      </c>
+      <c r="I54" s="30">
+        <v>-123.673425752431</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -4995,11 +5137,11 @@
       <c r="G55" s="30">
         <v>-123.81754599999999</v>
       </c>
-      <c r="H55" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I55" s="30" t="s">
-        <v>258</v>
+      <c r="H55" s="37">
+        <v>39.346401999999998</v>
+      </c>
+      <c r="I55" s="37">
+        <v>-123.754800707155</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -5022,11 +5164,11 @@
       <c r="G56" s="30">
         <v>-123.81754599999999</v>
       </c>
-      <c r="H56" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I56" s="30" t="s">
-        <v>258</v>
+      <c r="H56" s="30">
+        <v>39.346402108543899</v>
+      </c>
+      <c r="I56" s="30">
+        <v>-123.754800707158</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -5051,11 +5193,11 @@
       <c r="G57" s="30">
         <v>-123.794493</v>
       </c>
-      <c r="H57" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I57" s="30" t="s">
-        <v>258</v>
+      <c r="H57" s="37">
+        <v>39.33999</v>
+      </c>
+      <c r="I57" s="37">
+        <v>-123.595652201836</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -5080,11 +5222,11 @@
       <c r="G58" s="30">
         <v>-123.794493</v>
       </c>
-      <c r="H58" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I58" s="30" t="s">
-        <v>258</v>
+      <c r="H58" s="30">
+        <v>39.339990884676297</v>
+      </c>
+      <c r="I58" s="30">
+        <v>-123.595652201839</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -5107,11 +5249,11 @@
       <c r="G59" s="30">
         <v>-123.791837</v>
       </c>
-      <c r="H59" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I59" s="30" t="s">
-        <v>258</v>
+      <c r="H59" s="37">
+        <v>39.277107999999998</v>
+      </c>
+      <c r="I59" s="37">
+        <v>-123.742451353343</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -5134,11 +5276,11 @@
       <c r="G60" s="30">
         <v>-123.791837</v>
       </c>
-      <c r="H60" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I60" s="30" t="s">
-        <v>258</v>
+      <c r="H60" s="30">
+        <v>39.277108008857702</v>
+      </c>
+      <c r="I60" s="30">
+        <v>-123.742451353346</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -5161,11 +5303,11 @@
       <c r="G61" s="30">
         <v>-123.770308</v>
       </c>
-      <c r="H61" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I61" s="30" t="s">
-        <v>258</v>
+      <c r="H61" s="37">
+        <v>39.264657</v>
+      </c>
+      <c r="I61" s="37">
+        <v>-123.606849066691</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -5188,11 +5330,11 @@
       <c r="G62" s="30">
         <v>-123.770308</v>
       </c>
-      <c r="H62" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I62" s="30" t="s">
-        <v>258</v>
+      <c r="H62" s="30">
+        <v>39.264656917260702</v>
+      </c>
+      <c r="I62" s="30">
+        <v>-123.606849066694</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -5215,11 +5357,11 @@
       <c r="G63" s="30">
         <v>-123.769274</v>
       </c>
-      <c r="H63" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I63" s="30" t="s">
-        <v>258</v>
+      <c r="H63" s="37">
+        <v>39.200389000000001</v>
+      </c>
+      <c r="I63" s="37">
+        <v>-123.691288918997</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -5242,11 +5384,11 @@
       <c r="G64" s="30">
         <v>-123.769274</v>
       </c>
-      <c r="H64" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I64" s="30" t="s">
-        <v>258</v>
+      <c r="H64" s="30">
+        <v>39.200389268505901</v>
+      </c>
+      <c r="I64" s="30">
+        <v>-123.691288919</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -5271,11 +5413,11 @@
       <c r="G65" s="30">
         <v>-123.761134</v>
       </c>
-      <c r="H65" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I65" s="30" t="s">
-        <v>258</v>
+      <c r="H65" s="37">
+        <v>39.206978999999997</v>
+      </c>
+      <c r="I65" s="37">
+        <v>-123.536755275056</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -5300,11 +5442,11 @@
       <c r="G66" s="30">
         <v>-123.761134</v>
       </c>
-      <c r="H66" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I66" s="30" t="s">
-        <v>258</v>
+      <c r="H66" s="30">
+        <v>39.206979879401104</v>
+      </c>
+      <c r="I66" s="30">
+        <v>-123.536755275058</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -5318,7 +5460,7 @@
         <v>142</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>88</v>
+        <v>221</v>
       </c>
       <c r="E67" s="15" t="s">
         <v>89</v>
@@ -5329,11 +5471,11 @@
       <c r="G67" s="30">
         <v>-123.761134</v>
       </c>
-      <c r="H67" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I67" s="30" t="s">
-        <v>258</v>
+      <c r="H67" s="30">
+        <v>39.162621999999999</v>
+      </c>
+      <c r="I67" s="30">
+        <v>-123.582589</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -5350,7 +5492,7 @@
         <v>93</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>94</v>
+        <v>263</v>
       </c>
       <c r="F68" s="30">
         <v>38.954810000000002</v>
@@ -5358,11 +5500,11 @@
       <c r="G68" s="30">
         <v>-123.733526</v>
       </c>
-      <c r="H68" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I68" s="30" t="s">
-        <v>258</v>
+      <c r="H68" s="30">
+        <v>38.855753</v>
+      </c>
+      <c r="I68" s="30">
+        <v>-123.561122</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -5379,7 +5521,7 @@
         <v>93</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>95</v>
+        <v>264</v>
       </c>
       <c r="F69" s="30">
         <v>38.954810000000002</v>
@@ -5387,11 +5529,11 @@
       <c r="G69" s="30">
         <v>-123.733526</v>
       </c>
-      <c r="H69" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I69" s="30" t="s">
-        <v>258</v>
+      <c r="H69" s="30">
+        <v>38.928117999999998</v>
+      </c>
+      <c r="I69" s="30">
+        <v>-123.59921300000001</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -5414,11 +5556,11 @@
       <c r="G70" s="30">
         <v>-122.92983</v>
       </c>
-      <c r="H70" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I70" s="30" t="s">
-        <v>258</v>
+      <c r="H70" s="30">
+        <v>38.183169999999997</v>
+      </c>
+      <c r="I70" s="30">
+        <v>-122.83839</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -5441,11 +5583,11 @@
       <c r="G71" s="30">
         <v>-122.833217</v>
       </c>
-      <c r="H71" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I71" s="30" t="s">
-        <v>258</v>
+      <c r="H71" s="30">
+        <v>38.031847999999997</v>
+      </c>
+      <c r="I71" s="7">
+        <v>-122.74254614351401</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -5468,11 +5610,11 @@
       <c r="G72" s="30">
         <v>-122.833217</v>
       </c>
-      <c r="H72" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I72" s="30" t="s">
-        <v>258</v>
+      <c r="H72" s="30">
+        <v>38.034190000000002</v>
+      </c>
+      <c r="I72" s="30">
+        <v>-122.74263000000001</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -5497,11 +5639,11 @@
       <c r="G73" s="30">
         <v>-122.833217</v>
       </c>
-      <c r="H73" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I73" s="30" t="s">
-        <v>258</v>
+      <c r="H73" s="7">
+        <v>37.999115000000003</v>
+      </c>
+      <c r="I73" s="35">
+        <v>-122.755781559353</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -5526,11 +5668,11 @@
       <c r="G74" s="30">
         <v>-122.833217</v>
       </c>
-      <c r="H74" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I74" s="30" t="s">
-        <v>258</v>
+      <c r="H74" s="30">
+        <v>37.999115347780098</v>
+      </c>
+      <c r="I74" s="30">
+        <v>-122.755781559353</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -5555,11 +5697,11 @@
       <c r="G75" s="30">
         <v>-122.833217</v>
       </c>
-      <c r="H75" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I75" s="30" t="s">
-        <v>258</v>
+      <c r="H75" s="35">
+        <v>38.029805000000003</v>
+      </c>
+      <c r="I75" s="37">
+        <v>-122.735591284246</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -5584,11 +5726,11 @@
       <c r="G76" s="30">
         <v>-122.833217</v>
       </c>
-      <c r="H76" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I76" s="30" t="s">
-        <v>258</v>
+      <c r="H76" s="30">
+        <v>38.0298055212591</v>
+      </c>
+      <c r="I76" s="30">
+        <v>-122.735591284245</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -5611,11 +5753,11 @@
       <c r="G77" s="30">
         <v>-122.578053</v>
       </c>
-      <c r="H77" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I77" s="30" t="s">
-        <v>258</v>
+      <c r="H77" s="37">
+        <v>37.897621000000001</v>
+      </c>
+      <c r="I77" s="37">
+        <v>-122.57528166609499</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -5638,11 +5780,11 @@
       <c r="G78" s="30">
         <v>-122.578053</v>
       </c>
-      <c r="H78" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I78" s="30" t="s">
-        <v>258</v>
+      <c r="H78" s="30">
+        <v>37.884729999999998</v>
+      </c>
+      <c r="I78" s="30">
+        <v>-122.57051</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="15" customFormat="1">
@@ -5665,11 +5807,11 @@
       <c r="G79" s="3">
         <v>-122.230897</v>
       </c>
-      <c r="H79" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I79" s="30" t="s">
-        <v>258</v>
+      <c r="H79" s="37">
+        <v>37.040588999999997</v>
+      </c>
+      <c r="I79" s="7">
+        <v>-122.228973455241</v>
       </c>
     </row>
     <row r="80" spans="1:9" s="15" customFormat="1">
@@ -5692,14 +5834,17 @@
       <c r="G80" s="3">
         <v>-122.230897</v>
       </c>
-      <c r="H80" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I80" s="30" t="s">
-        <v>258</v>
+      <c r="H80" s="30">
+        <v>37.045313</v>
+      </c>
+      <c r="I80" s="30">
+        <v>-122.22650400000001</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:I80">
+    <sortCondition ref="A2:A80"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -5715,7 +5860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection sqref="A1:G48"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Merged EHUa population into EHTa (as in TRT paper), because these samples were collected in almost the same location just a few days-weeks apart, and thus could contain siblings.  Three files modified to reflect these changes.
</commit_message>
<xml_diff>
--- a/data/coho_coastw_pops_N_S.xlsx
+++ b/data/coho_coastw_pops_N_S.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="160" windowWidth="26900" windowHeight="25860" tabRatio="500"/>
+    <workbookView xWindow="2040" yWindow="100" windowWidth="32640" windowHeight="26520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="N-S by pop code" sheetId="5" r:id="rId1"/>
@@ -642,7 +642,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="H40" authorId="0">
+    <comment ref="A39" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+NS039 was combined with NS038 050916</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B39" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+EHUa combined with EHTa b/c samples collected at almost same site just few weeks apart (these pops wer combined for TRT paper) 050916</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H39" authorId="0">
       <text>
         <r>
           <rPr>
@@ -666,7 +714,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I40" authorId="0">
+    <comment ref="I39" authorId="0">
       <text>
         <r>
           <rPr>
@@ -687,6 +735,30 @@
           </rPr>
           <t xml:space="preserve">
 per Tommy on TRT data, two HT sites were almost on top of each other, so treat as a single pop.  EHTa and EHUa should be combined for most analysis 050616</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F67" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+mouth is just north of Point Arena</t>
         </r>
       </text>
     </comment>
@@ -734,7 +806,31 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-mouth is just north of Point Arena</t>
+coords taken where Walker Ck meets Tomales Bay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B70" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+low n, to drop?</t>
         </r>
       </text>
     </comment>
@@ -758,31 +854,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-coords taken where Walker Ck meets Tomales Bay</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B71" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Libby Gilbert-Horvath:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-low n, to drop?</t>
+coords taken where Lagunitas delta meets Tomales Bay</t>
         </r>
       </text>
     </comment>
@@ -906,31 +978,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F76" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Libby Gilbert-Horvath:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-coords taken where Lagunitas delta meets Tomales Bay</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B77" authorId="0">
+    <comment ref="B76" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1314,7 +1362,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="262">
   <si>
     <t>Noyo River</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -1923,12 +1971,6 @@
     <t>KSSb and KSHb</t>
   </si>
   <si>
-    <t>EHTa and EHUa</t>
-  </si>
-  <si>
-    <t>Hollow Tree Creek and Upper HT Ck</t>
-  </si>
-  <si>
     <t>not visited</t>
   </si>
   <si>
@@ -1995,16 +2037,10 @@
     <t>N-S_order</t>
   </si>
   <si>
-    <t>EHUa</t>
-  </si>
-  <si>
     <t>EHTa</t>
   </si>
   <si>
     <t>Hollow Tree Creek</t>
-  </si>
-  <si>
-    <t>Upper Hollow Tree Creek</t>
   </si>
   <si>
     <t>Rogue R Illinois River</t>
@@ -2164,7 +2200,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -2255,11 +2291,6 @@
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="9" tint="-0.499984740745262"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2299,7 +2330,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="419">
+  <cellStyleXfs count="421">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2719,8 +2750,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2795,11 +2828,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="419">
+  <cellStyles count="421">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3009,6 +3039,7 @@
     <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3218,6 +3249,7 @@
     <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3547,11 +3579,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3559,20 +3591,20 @@
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="7" width="13.42578125" style="30" customWidth="1"/>
     <col min="8" max="9" width="16.42578125" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" customHeight="1">
       <c r="A1" s="21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -3581,16 +3613,16 @@
         <v>7</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3662,7 +3694,7 @@
         <v>142</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>118</v>
@@ -3691,7 +3723,7 @@
         <v>142</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>119</v>
@@ -3749,7 +3781,7 @@
         <v>142</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>116</v>
@@ -3778,7 +3810,7 @@
         <v>142</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>113</v>
@@ -3807,7 +3839,7 @@
         <v>142</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>114</v>
@@ -3933,7 +3965,7 @@
         <v>41.647773000000001</v>
       </c>
       <c r="I13" s="33" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3950,7 +3982,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F14" s="30">
         <v>41.542819999999999</v>
@@ -3979,7 +4011,7 @@
         <v>9</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F15" s="30">
         <v>41.542819999999999</v>
@@ -4144,7 +4176,7 @@
         <v>162</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>140</v>
@@ -4173,7 +4205,7 @@
         <v>163</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>142</v>
@@ -4202,7 +4234,7 @@
         <v>164</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>141</v>
@@ -4231,7 +4263,7 @@
         <v>165</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C24" s="23" t="s">
         <v>185</v>
@@ -4556,7 +4588,7 @@
         <v>140</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>29</v>
@@ -4585,7 +4617,7 @@
         <v>142</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>29</v>
@@ -4614,10 +4646,10 @@
         <v>140</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F37" s="30">
         <v>40.767724000000001</v>
@@ -4643,10 +4675,10 @@
         <v>142</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F38" s="30">
         <v>40.767724000000001</v>
@@ -4666,16 +4698,16 @@
         <v>180</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>140</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F39" s="30">
         <v>40.649000999999998</v>
@@ -4692,19 +4724,19 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>140</v>
+        <v>61</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F40" s="30">
         <v>40.649000999999998</v>
@@ -4712,138 +4744,136 @@
       <c r="G40" s="30">
         <v>-124.30950300000001</v>
       </c>
-      <c r="H40" s="38">
-        <v>39.739350000000002</v>
-      </c>
-      <c r="I40" s="38">
-        <v>-123.719786158689</v>
+      <c r="H40" s="30">
+        <v>39.373964999999998</v>
+      </c>
+      <c r="I40" s="30">
+        <v>-123.719786</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="15" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>142</v>
+        <v>62</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="F41" s="30">
-        <v>40.649000999999998</v>
-      </c>
-      <c r="G41" s="30">
-        <v>-124.30950300000001</v>
-      </c>
-      <c r="H41" s="30">
-        <v>39.373964999999998</v>
-      </c>
-      <c r="I41" s="30">
-        <v>-123.719786</v>
+        <v>256</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="F41" s="3">
+        <v>40.302202999999999</v>
+      </c>
+      <c r="G41" s="3">
+        <v>-124.35406999999999</v>
+      </c>
+      <c r="H41" s="35">
+        <v>39.993645000000001</v>
+      </c>
+      <c r="I41" s="35">
+        <v>-123.924254484123</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="F42" s="3">
+        <v>189</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="F42" s="5">
         <v>40.302202999999999</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="5">
         <v>-124.35406999999999</v>
       </c>
-      <c r="H42" s="35">
-        <v>39.993645000000001</v>
-      </c>
-      <c r="I42" s="35">
-        <v>-123.924254484123</v>
+      <c r="H42" s="5">
+        <v>40.008785000000003</v>
+      </c>
+      <c r="I42" s="5">
+        <v>-123.93082699999999</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" s="30">
+        <v>39.736032000000002</v>
+      </c>
+      <c r="G43" s="30">
+        <v>-123.829384</v>
+      </c>
+      <c r="H43" s="37">
+        <v>39.737169000000002</v>
+      </c>
+      <c r="I43" s="37">
+        <v>-123.811457138802</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B43" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="F43" s="5">
-        <v>40.302202999999999</v>
-      </c>
-      <c r="G43" s="5">
-        <v>-124.35406999999999</v>
-      </c>
-      <c r="H43" s="5">
-        <v>40.008785000000003</v>
-      </c>
-      <c r="I43" s="5">
-        <v>-123.93082699999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="15" t="s">
-        <v>192</v>
-      </c>
       <c r="B44" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>140</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E44" s="3"/>
       <c r="F44" s="30">
-        <v>39.736032000000002</v>
+        <v>39.651716</v>
       </c>
       <c r="G44" s="30">
-        <v>-123.829384</v>
+        <v>-123.785082</v>
       </c>
       <c r="H44" s="37">
-        <v>39.737169000000002</v>
+        <v>39.646847999999999</v>
       </c>
       <c r="I44" s="37">
-        <v>-123.811457138802</v>
+        <v>-123.739059359408</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>140</v>
+        <v>67</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>25</v>
@@ -4855,55 +4885,57 @@
       <c r="G45" s="30">
         <v>-123.785082</v>
       </c>
-      <c r="H45" s="37">
-        <v>39.646847999999999</v>
-      </c>
-      <c r="I45" s="37">
-        <v>-123.739059359408</v>
+      <c r="H45" s="30">
+        <v>39.6468482090145</v>
+      </c>
+      <c r="I45" s="30">
+        <v>-123.739059359411</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="F46" s="30">
+        <v>39.553401999999998</v>
+      </c>
+      <c r="G46" s="30">
+        <v>-123.76682599999999</v>
+      </c>
+      <c r="H46" s="37">
+        <v>39.593316999999999</v>
+      </c>
+      <c r="I46" s="37">
+        <v>-123.71178554974099</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="B46" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="30">
-        <v>39.651716</v>
-      </c>
-      <c r="G46" s="30">
-        <v>-123.785082</v>
-      </c>
-      <c r="H46" s="30">
-        <v>39.6468482090145</v>
-      </c>
-      <c r="I46" s="30">
-        <v>-123.739059359411</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>140</v>
+      <c r="B47" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F47" s="30">
         <v>39.553401999999998</v>
@@ -4911,19 +4943,19 @@
       <c r="G47" s="30">
         <v>-123.76682599999999</v>
       </c>
-      <c r="H47" s="37">
-        <v>39.593316999999999</v>
-      </c>
-      <c r="I47" s="37">
-        <v>-123.71178554974099</v>
+      <c r="H47" s="30">
+        <v>39.593317417398701</v>
+      </c>
+      <c r="I47" s="30">
+        <v>-123.71178554974399</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="15" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>142</v>
@@ -4932,7 +4964,7 @@
         <v>26</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>262</v>
+        <v>70</v>
       </c>
       <c r="F48" s="30">
         <v>39.553401999999998</v>
@@ -4941,18 +4973,18 @@
         <v>-123.76682599999999</v>
       </c>
       <c r="H48" s="30">
-        <v>39.593317417398701</v>
+        <v>39.515115999999999</v>
       </c>
       <c r="I48" s="30">
-        <v>-123.71178554974399</v>
+        <v>-123.707942</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="15" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>142</v>
@@ -4961,7 +4993,7 @@
         <v>26</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F49" s="30">
         <v>39.553401999999998</v>
@@ -4970,50 +5002,48 @@
         <v>-123.76682599999999</v>
       </c>
       <c r="H49" s="30">
-        <v>39.515115999999999</v>
+        <v>39.503129000000001</v>
       </c>
       <c r="I49" s="30">
-        <v>-123.707942</v>
+        <v>-123.610786</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>142</v>
+        <v>220</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>72</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E50" s="3"/>
       <c r="F50" s="30">
-        <v>39.553401999999998</v>
+        <v>39.459125</v>
       </c>
       <c r="G50" s="30">
-        <v>-123.76682599999999</v>
-      </c>
-      <c r="H50" s="30">
-        <v>39.503129000000001</v>
-      </c>
-      <c r="I50" s="30">
-        <v>-123.610786</v>
+        <v>-123.80941199999999</v>
+      </c>
+      <c r="H50" s="37">
+        <v>39.467663000000002</v>
+      </c>
+      <c r="I50" s="37">
+        <v>-123.72560470636201</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="B51" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>140</v>
+        <v>221</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>27</v>
@@ -5025,49 +5055,51 @@
       <c r="G51" s="30">
         <v>-123.80941199999999</v>
       </c>
-      <c r="H51" s="37">
-        <v>39.467663000000002</v>
-      </c>
-      <c r="I51" s="37">
-        <v>-123.72560470636201</v>
+      <c r="H51" s="30">
+        <v>39.467663053255897</v>
+      </c>
+      <c r="I51" s="30">
+        <v>-123.725604706365</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>142</v>
+        <v>222</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F52" s="30">
-        <v>39.459125</v>
+        <v>39.427914000000001</v>
       </c>
       <c r="G52" s="30">
-        <v>-123.80941199999999</v>
-      </c>
-      <c r="H52" s="30">
-        <v>39.467663053255897</v>
-      </c>
-      <c r="I52" s="30">
-        <v>-123.725604706365</v>
+        <v>-123.810671</v>
+      </c>
+      <c r="H52" s="37">
+        <v>39.383845000000001</v>
+      </c>
+      <c r="I52" s="37">
+        <v>-123.673425752428</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="B53" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>140</v>
+        <v>223</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>0</v>
@@ -5081,51 +5113,49 @@
       <c r="G53" s="30">
         <v>-123.810671</v>
       </c>
-      <c r="H53" s="37">
-        <v>39.383845000000001</v>
-      </c>
-      <c r="I53" s="37">
-        <v>-123.673425752428</v>
+      <c r="H53" s="30">
+        <v>39.3838452552584</v>
+      </c>
+      <c r="I53" s="30">
+        <v>-123.673425752431</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>142</v>
+        <v>224</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E54" s="3"/>
       <c r="F54" s="30">
-        <v>39.427914000000001</v>
+        <v>39.361863999999997</v>
       </c>
       <c r="G54" s="30">
-        <v>-123.810671</v>
-      </c>
-      <c r="H54" s="30">
-        <v>39.3838452552584</v>
-      </c>
-      <c r="I54" s="30">
-        <v>-123.673425752431</v>
+        <v>-123.81754599999999</v>
+      </c>
+      <c r="H54" s="37">
+        <v>39.346401999999998</v>
+      </c>
+      <c r="I54" s="37">
+        <v>-123.754800707155</v>
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>140</v>
+      <c r="A55" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>1</v>
@@ -5137,49 +5167,51 @@
       <c r="G55" s="30">
         <v>-123.81754599999999</v>
       </c>
-      <c r="H55" s="37">
-        <v>39.346401999999998</v>
-      </c>
-      <c r="I55" s="37">
-        <v>-123.754800707155</v>
+      <c r="H55" s="30">
+        <v>39.346402108543899</v>
+      </c>
+      <c r="I55" s="30">
+        <v>-123.754800707158</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C56" s="18" t="s">
-        <v>142</v>
+        <v>226</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E56" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="F56" s="30">
-        <v>39.361863999999997</v>
+        <v>39.302027000000002</v>
       </c>
       <c r="G56" s="30">
-        <v>-123.81754599999999</v>
-      </c>
-      <c r="H56" s="30">
-        <v>39.346402108543899</v>
-      </c>
-      <c r="I56" s="30">
-        <v>-123.754800707158</v>
+        <v>-123.794493</v>
+      </c>
+      <c r="H56" s="37">
+        <v>39.33999</v>
+      </c>
+      <c r="I56" s="37">
+        <v>-123.595652201836</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>140</v>
+        <v>227</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>2</v>
@@ -5193,51 +5225,49 @@
       <c r="G57" s="30">
         <v>-123.794493</v>
       </c>
-      <c r="H57" s="37">
-        <v>39.33999</v>
-      </c>
-      <c r="I57" s="37">
-        <v>-123.595652201836</v>
+      <c r="H57" s="30">
+        <v>39.339990884676297</v>
+      </c>
+      <c r="I57" s="30">
+        <v>-123.595652201839</v>
       </c>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C58" s="18" t="s">
-        <v>142</v>
+      <c r="A58" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>3</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E58" s="3"/>
       <c r="F58" s="30">
-        <v>39.302027000000002</v>
+        <v>39.273693000000002</v>
       </c>
       <c r="G58" s="30">
-        <v>-123.794493</v>
-      </c>
-      <c r="H58" s="30">
-        <v>39.339990884676297</v>
-      </c>
-      <c r="I58" s="30">
-        <v>-123.595652201839</v>
+        <v>-123.791837</v>
+      </c>
+      <c r="H58" s="37">
+        <v>39.277107999999998</v>
+      </c>
+      <c r="I58" s="37">
+        <v>-123.742451353343</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>140</v>
+        <v>229</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>20</v>
@@ -5249,103 +5279,103 @@
       <c r="G59" s="30">
         <v>-123.791837</v>
       </c>
-      <c r="H59" s="37">
-        <v>39.277107999999998</v>
-      </c>
-      <c r="I59" s="37">
-        <v>-123.742451353343</v>
+      <c r="H59" s="30">
+        <v>39.277108008857702</v>
+      </c>
+      <c r="I59" s="30">
+        <v>-123.742451353346</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C60" s="18" t="s">
-        <v>142</v>
+        <v>230</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="30">
-        <v>39.273693000000002</v>
+        <v>39.226984999999999</v>
       </c>
       <c r="G60" s="30">
-        <v>-123.791837</v>
-      </c>
-      <c r="H60" s="30">
-        <v>39.277108008857702</v>
-      </c>
-      <c r="I60" s="30">
-        <v>-123.742451353346</v>
+        <v>-123.770308</v>
+      </c>
+      <c r="H60" s="37">
+        <v>39.264657</v>
+      </c>
+      <c r="I60" s="37">
+        <v>-123.606849066691</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="B61" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>140</v>
+        <v>231</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E61" s="3"/>
+      <c r="E61" s="18"/>
       <c r="F61" s="30">
         <v>39.226984999999999</v>
       </c>
       <c r="G61" s="30">
         <v>-123.770308</v>
       </c>
-      <c r="H61" s="37">
-        <v>39.264657</v>
-      </c>
-      <c r="I61" s="37">
-        <v>-123.606849066691</v>
+      <c r="H61" s="30">
+        <v>39.264656917260702</v>
+      </c>
+      <c r="I61" s="30">
+        <v>-123.606849066694</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>142</v>
+        <v>232</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E62" s="18"/>
+        <v>5</v>
+      </c>
+      <c r="E62" s="3"/>
       <c r="F62" s="30">
-        <v>39.226984999999999</v>
+        <v>39.215594000000003</v>
       </c>
       <c r="G62" s="30">
-        <v>-123.770308</v>
-      </c>
-      <c r="H62" s="30">
-        <v>39.264656917260702</v>
-      </c>
-      <c r="I62" s="30">
-        <v>-123.606849066694</v>
+        <v>-123.769274</v>
+      </c>
+      <c r="H62" s="37">
+        <v>39.200389000000001</v>
+      </c>
+      <c r="I62" s="37">
+        <v>-123.691288918997</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="B63" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>140</v>
+        <v>233</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>5</v>
@@ -5357,52 +5387,54 @@
       <c r="G63" s="30">
         <v>-123.769274</v>
       </c>
-      <c r="H63" s="37">
-        <v>39.200389000000001</v>
-      </c>
-      <c r="I63" s="37">
-        <v>-123.691288918997</v>
+      <c r="H63" s="30">
+        <v>39.200389268505901</v>
+      </c>
+      <c r="I63" s="30">
+        <v>-123.691288919</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C64" s="18" t="s">
-        <v>142</v>
+        <v>234</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E64" s="3"/>
+        <v>217</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="F64" s="30">
-        <v>39.215594000000003</v>
+        <v>39.191763000000002</v>
       </c>
       <c r="G64" s="30">
-        <v>-123.769274</v>
-      </c>
-      <c r="H64" s="30">
-        <v>39.200389268505901</v>
-      </c>
-      <c r="I64" s="30">
-        <v>-123.691288919</v>
+        <v>-123.761134</v>
+      </c>
+      <c r="H64" s="37">
+        <v>39.206978999999997</v>
+      </c>
+      <c r="I64" s="37">
+        <v>-123.536755275056</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="B65" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>140</v>
+        <v>235</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>38</v>
@@ -5413,28 +5445,28 @@
       <c r="G65" s="30">
         <v>-123.761134</v>
       </c>
-      <c r="H65" s="37">
-        <v>39.206978999999997</v>
-      </c>
-      <c r="I65" s="37">
-        <v>-123.536755275056</v>
+      <c r="H65" s="30">
+        <v>39.206979879401104</v>
+      </c>
+      <c r="I65" s="30">
+        <v>-123.536755275058</v>
       </c>
     </row>
     <row r="66" spans="1:9">
-      <c r="A66" s="15" t="s">
-        <v>239</v>
+      <c r="A66" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C66" s="18" t="s">
         <v>142</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>38</v>
+        <v>217</v>
+      </c>
+      <c r="E66" s="15" t="s">
+        <v>89</v>
       </c>
       <c r="F66" s="30">
         <v>39.191763000000002</v>
@@ -5443,47 +5475,47 @@
         <v>-123.761134</v>
       </c>
       <c r="H66" s="30">
-        <v>39.206979879401104</v>
+        <v>39.162621999999999</v>
       </c>
       <c r="I66" s="30">
-        <v>-123.536755275058</v>
+        <v>-123.582589</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>92</v>
+        <v>129</v>
       </c>
       <c r="C67" s="18" t="s">
         <v>142</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E67" s="15" t="s">
-        <v>89</v>
+        <v>93</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>259</v>
       </c>
       <c r="F67" s="30">
-        <v>39.191763000000002</v>
+        <v>38.954810000000002</v>
       </c>
       <c r="G67" s="30">
-        <v>-123.761134</v>
+        <v>-123.733526</v>
       </c>
       <c r="H67" s="30">
-        <v>39.162621999999999</v>
+        <v>38.855753</v>
       </c>
       <c r="I67" s="30">
-        <v>-123.582589</v>
+        <v>-123.561122</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C68" s="18" t="s">
         <v>142</v>
@@ -5491,8 +5523,8 @@
       <c r="D68" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E68" s="8" t="s">
-        <v>263</v>
+      <c r="E68" s="7" t="s">
+        <v>260</v>
       </c>
       <c r="F68" s="30">
         <v>38.954810000000002</v>
@@ -5501,77 +5533,75 @@
         <v>-123.733526</v>
       </c>
       <c r="H68" s="30">
-        <v>38.855753</v>
+        <v>38.928117999999998</v>
       </c>
       <c r="I68" s="30">
-        <v>-123.561122</v>
+        <v>-123.59921300000001</v>
       </c>
     </row>
     <row r="69" spans="1:9">
-      <c r="A69" s="1" t="s">
-        <v>242</v>
+      <c r="A69" s="15" t="s">
+        <v>239</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C69" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>264</v>
-      </c>
+      <c r="D69" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E69" s="15"/>
       <c r="F69" s="30">
-        <v>38.954810000000002</v>
+        <v>38.209601999999997</v>
       </c>
       <c r="G69" s="30">
-        <v>-123.733526</v>
+        <v>-122.92983</v>
       </c>
       <c r="H69" s="30">
-        <v>38.928117999999998</v>
+        <v>38.183169999999997</v>
       </c>
       <c r="I69" s="30">
-        <v>-123.59921300000001</v>
+        <v>-122.83839</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="B70" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C70" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E70" s="15"/>
+        <v>240</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E70" s="3"/>
       <c r="F70" s="30">
-        <v>38.209601999999997</v>
+        <v>38.089637000000003</v>
       </c>
       <c r="G70" s="30">
-        <v>-122.92983</v>
+        <v>-122.833217</v>
       </c>
       <c r="H70" s="30">
-        <v>38.183169999999997</v>
-      </c>
-      <c r="I70" s="30">
-        <v>-122.83839</v>
+        <v>38.031847999999997</v>
+      </c>
+      <c r="I70" s="7">
+        <v>-122.74254614351401</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>140</v>
+        <v>241</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>32</v>
@@ -5584,48 +5614,50 @@
         <v>-122.833217</v>
       </c>
       <c r="H71" s="30">
-        <v>38.031847999999997</v>
-      </c>
-      <c r="I71" s="7">
-        <v>-122.74254614351401</v>
+        <v>38.034190000000002</v>
+      </c>
+      <c r="I71" s="30">
+        <v>-122.74263000000001</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C72" s="18" t="s">
-        <v>142</v>
+        <v>242</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E72" s="3"/>
+      <c r="E72" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="F72" s="30">
         <v>38.089637000000003</v>
       </c>
       <c r="G72" s="30">
         <v>-122.833217</v>
       </c>
-      <c r="H72" s="30">
-        <v>38.034190000000002</v>
-      </c>
-      <c r="I72" s="30">
-        <v>-122.74263000000001</v>
+      <c r="H72" s="7">
+        <v>37.999115000000003</v>
+      </c>
+      <c r="I72" s="35">
+        <v>-122.755781559353</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="B73" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>140</v>
+        <v>243</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>32</v>
@@ -5639,28 +5671,28 @@
       <c r="G73" s="30">
         <v>-122.833217</v>
       </c>
-      <c r="H73" s="7">
-        <v>37.999115000000003</v>
-      </c>
-      <c r="I73" s="35">
+      <c r="H73" s="30">
+        <v>37.999115347780098</v>
+      </c>
+      <c r="I73" s="30">
         <v>-122.755781559353</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="B74" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C74" s="18" t="s">
-        <v>142</v>
+        <v>244</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F74" s="30">
         <v>38.089637000000003</v>
@@ -5668,22 +5700,22 @@
       <c r="G74" s="30">
         <v>-122.833217</v>
       </c>
-      <c r="H74" s="30">
-        <v>37.999115347780098</v>
-      </c>
-      <c r="I74" s="30">
-        <v>-122.755781559353</v>
+      <c r="H74" s="35">
+        <v>38.029805000000003</v>
+      </c>
+      <c r="I74" s="37">
+        <v>-122.735591284246</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="B75" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>140</v>
+        <v>245</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>32</v>
@@ -5697,51 +5729,49 @@
       <c r="G75" s="30">
         <v>-122.833217</v>
       </c>
-      <c r="H75" s="35">
-        <v>38.029805000000003</v>
-      </c>
-      <c r="I75" s="37">
-        <v>-122.735591284246</v>
+      <c r="H75" s="30">
+        <v>38.0298055212591</v>
+      </c>
+      <c r="I75" s="30">
+        <v>-122.735591284245</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C76" s="18" t="s">
-        <v>142</v>
+        <v>246</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>34</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E76" s="3"/>
       <c r="F76" s="30">
-        <v>38.089637000000003</v>
+        <v>37.859591999999999</v>
       </c>
       <c r="G76" s="30">
-        <v>-122.833217</v>
-      </c>
-      <c r="H76" s="30">
-        <v>38.0298055212591</v>
-      </c>
-      <c r="I76" s="30">
-        <v>-122.735591284245</v>
+        <v>-122.578053</v>
+      </c>
+      <c r="H76" s="37">
+        <v>37.897621000000001</v>
+      </c>
+      <c r="I76" s="37">
+        <v>-122.57528166609499</v>
       </c>
     </row>
     <row r="77" spans="1:9">
-      <c r="A77" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="B77" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>140</v>
+      <c r="A77" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>16</v>
@@ -5753,91 +5783,64 @@
       <c r="G77" s="30">
         <v>-122.578053</v>
       </c>
-      <c r="H77" s="37">
-        <v>37.897621000000001</v>
-      </c>
-      <c r="I77" s="37">
-        <v>-122.57528166609499</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="H77" s="30">
+        <v>37.884729999999998</v>
+      </c>
+      <c r="I77" s="30">
+        <v>-122.57051</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" s="15" customFormat="1">
       <c r="A78" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C78" s="18" t="s">
-        <v>142</v>
+        <v>248</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="E78" s="3"/>
-      <c r="F78" s="30">
-        <v>37.859591999999999</v>
-      </c>
-      <c r="G78" s="30">
-        <v>-122.578053</v>
-      </c>
-      <c r="H78" s="30">
-        <v>37.884729999999998</v>
-      </c>
-      <c r="I78" s="30">
-        <v>-122.57051</v>
+      <c r="F78" s="3">
+        <v>37.041151999999997</v>
+      </c>
+      <c r="G78" s="3">
+        <v>-122.230897</v>
+      </c>
+      <c r="H78" s="37">
+        <v>37.040588999999997</v>
+      </c>
+      <c r="I78" s="7">
+        <v>-122.228973455241</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="15" customFormat="1">
       <c r="A79" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>140</v>
+        <v>105</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E79" s="3"/>
+      <c r="E79" s="18"/>
       <c r="F79" s="3">
         <v>37.041151999999997</v>
       </c>
       <c r="G79" s="3">
         <v>-122.230897</v>
       </c>
-      <c r="H79" s="37">
-        <v>37.040588999999997</v>
-      </c>
-      <c r="I79" s="7">
-        <v>-122.228973455241</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" s="15" customFormat="1">
-      <c r="A80" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B80" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C80" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E80" s="18"/>
-      <c r="F80" s="3">
-        <v>37.041151999999997</v>
-      </c>
-      <c r="G80" s="3">
-        <v>-122.230897</v>
-      </c>
-      <c r="H80" s="30">
+      <c r="H79" s="30">
         <v>37.045313</v>
       </c>
-      <c r="I80" s="30">
+      <c r="I79" s="30">
         <v>-122.22650400000001</v>
       </c>
     </row>
@@ -5861,7 +5864,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:G48"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5877,19 +5880,19 @@
   <sheetData>
     <row r="1" spans="1:7" s="20" customFormat="1" ht="52" customHeight="1">
       <c r="A1" s="21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D1" s="28" t="s">
         <v>40</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
@@ -5903,7 +5906,7 @@
         <v>143</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>36</v>
@@ -5926,7 +5929,7 @@
         <v>144</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>36</v>
@@ -5949,7 +5952,7 @@
         <v>145</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>36</v>
@@ -5972,7 +5975,7 @@
         <v>146</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>36</v>
@@ -5995,7 +5998,7 @@
         <v>147</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>36</v>
@@ -6018,7 +6021,7 @@
         <v>148</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>36</v>
@@ -6041,7 +6044,7 @@
         <v>149</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>36</v>
@@ -6064,7 +6067,7 @@
         <v>150</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>36</v>
@@ -6087,7 +6090,7 @@
         <v>151</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>36</v>
@@ -6110,7 +6113,7 @@
         <v>152</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>36</v>
@@ -6169,7 +6172,7 @@
         <v>9</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="15" customFormat="1">
@@ -6249,13 +6252,13 @@
         <v>186</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>187</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>37</v>
@@ -6419,10 +6422,10 @@
         <v>142</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="15" customFormat="1">
@@ -6430,7 +6433,7 @@
         <v>166</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>140</v>
@@ -6445,7 +6448,7 @@
         <v>31</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="15" customFormat="1">
@@ -6533,7 +6536,7 @@
         <v>26</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="15" customFormat="1">
@@ -6827,7 +6830,7 @@
     </row>
     <row r="43" spans="1:7" s="15" customFormat="1">
       <c r="A43" s="15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>64</v>
@@ -6847,7 +6850,7 @@
     </row>
     <row r="44" spans="1:7" s="15" customFormat="1">
       <c r="A44" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>97</v>
@@ -6868,7 +6871,7 @@
     </row>
     <row r="45" spans="1:7" s="15" customFormat="1">
       <c r="A45" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>98</v>
@@ -6891,7 +6894,7 @@
     </row>
     <row r="46" spans="1:7" s="15" customFormat="1">
       <c r="A46" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B46" s="16" t="s">
         <v>100</v>
@@ -6914,7 +6917,7 @@
     </row>
     <row r="47" spans="1:7" s="15" customFormat="1">
       <c r="A47" s="15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B47" s="16" t="s">
         <v>102</v>
@@ -6935,7 +6938,7 @@
     </row>
     <row r="48" spans="1:7" s="15" customFormat="1">
       <c r="A48" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>104</v>

</xml_diff>